<commit_message>
correct weight update error
</commit_message>
<xml_diff>
--- a/app/outputs/partner-solver-init-weights.xlsx
+++ b/app/outputs/partner-solver-init-weights.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Partner Solver Weights" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2570" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2570" uniqueCount="80">
   <si>
     <t>Org_y</t>
   </si>
@@ -250,13 +250,10 @@
     <t>change:WATER Labs' iThrone: a waste-shrinking toilet</t>
   </si>
   <si>
-    <t>12</t>
+    <t>2</t>
   </si>
   <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>3</t>
   </si>
 </sst>
 </file>
@@ -1111,13 +1108,13 @@
         <v>1</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1247,17 +1244,17 @@
       <c r="B32" t="s">
         <v>46</v>
       </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-      <c r="F32">
-        <v>1</v>
+      <c r="C32" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32" t="s">
+        <v>79</v>
+      </c>
+      <c r="F32" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2051,13 +2048,13 @@
         <v>1</v>
       </c>
       <c r="D72">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E72">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F72">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -12311,10 +12308,10 @@
         <v>1</v>
       </c>
       <c r="D585">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E585">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F585">
         <v>1</v>
@@ -15507,17 +15504,17 @@
       <c r="B745" t="s">
         <v>64</v>
       </c>
-      <c r="C745" t="s">
-        <v>78</v>
-      </c>
-      <c r="D745" t="s">
-        <v>79</v>
-      </c>
-      <c r="E745" t="s">
-        <v>80</v>
-      </c>
-      <c r="F745" t="s">
-        <v>79</v>
+      <c r="C745">
+        <v>1</v>
+      </c>
+      <c r="D745">
+        <v>1</v>
+      </c>
+      <c r="E745">
+        <v>1</v>
+      </c>
+      <c r="F745">
+        <v>1</v>
       </c>
     </row>
     <row r="746" spans="1:6">

</xml_diff>

<commit_message>
added color change on partner table
</commit_message>
<xml_diff>
--- a/app/outputs/partner-solver-init-weights.xlsx
+++ b/app/outputs/partner-solver-init-weights.xlsx
@@ -2558,17 +2558,17 @@
       <c r="B98" t="s">
         <v>47</v>
       </c>
-      <c r="C98">
-        <v>1</v>
-      </c>
-      <c r="D98">
-        <v>1</v>
-      </c>
-      <c r="E98">
-        <v>1</v>
-      </c>
-      <c r="F98">
-        <v>1</v>
+      <c r="C98" t="s">
+        <v>77</v>
+      </c>
+      <c r="D98" t="s">
+        <v>77</v>
+      </c>
+      <c r="E98" t="s">
+        <v>77</v>
+      </c>
+      <c r="F98" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -2778,17 +2778,17 @@
       <c r="B109" t="s">
         <v>47</v>
       </c>
-      <c r="C109" t="s">
-        <v>77</v>
-      </c>
-      <c r="D109" t="s">
-        <v>77</v>
-      </c>
-      <c r="E109" t="s">
-        <v>77</v>
-      </c>
-      <c r="F109" t="s">
-        <v>77</v>
+      <c r="C109">
+        <v>1</v>
+      </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
+      <c r="E109">
+        <v>1</v>
+      </c>
+      <c r="F109">
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:6">

</xml_diff>

<commit_message>
adding log level for debugging
</commit_message>
<xml_diff>
--- a/app/outputs/partner-solver-init-weights.xlsx
+++ b/app/outputs/partner-solver-init-weights.xlsx
@@ -2878,17 +2878,17 @@
       <c r="B114" t="s">
         <v>47</v>
       </c>
-      <c r="C114" t="s">
-        <v>77</v>
-      </c>
-      <c r="D114" t="s">
-        <v>77</v>
-      </c>
-      <c r="E114" t="s">
-        <v>77</v>
-      </c>
-      <c r="F114" t="s">
-        <v>77</v>
+      <c r="C114">
+        <v>1</v>
+      </c>
+      <c r="D114">
+        <v>1</v>
+      </c>
+      <c r="E114">
+        <v>1</v>
+      </c>
+      <c r="F114">
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -12058,17 +12058,17 @@
       <c r="B573" t="s">
         <v>59</v>
       </c>
-      <c r="C573">
-        <v>1</v>
-      </c>
-      <c r="D573">
-        <v>1</v>
-      </c>
-      <c r="E573">
-        <v>1</v>
-      </c>
-      <c r="F573">
-        <v>1</v>
+      <c r="C573" t="s">
+        <v>77</v>
+      </c>
+      <c r="D573" t="s">
+        <v>77</v>
+      </c>
+      <c r="E573" t="s">
+        <v>77</v>
+      </c>
+      <c r="F573" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="574" spans="1:6">

</xml_diff>

<commit_message>
turn off individual plot on dropdown change
</commit_message>
<xml_diff>
--- a/app/outputs/partner-solver-init-weights.xlsx
+++ b/app/outputs/partner-solver-init-weights.xlsx
@@ -2638,17 +2638,17 @@
       <c r="B102" t="s">
         <v>47</v>
       </c>
-      <c r="C102">
-        <v>1</v>
-      </c>
-      <c r="D102">
-        <v>1</v>
-      </c>
-      <c r="E102">
-        <v>1</v>
-      </c>
-      <c r="F102">
-        <v>1</v>
+      <c r="C102" t="s">
+        <v>77</v>
+      </c>
+      <c r="D102" t="s">
+        <v>77</v>
+      </c>
+      <c r="E102" t="s">
+        <v>77</v>
+      </c>
+      <c r="F102" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -15298,17 +15298,17 @@
       <c r="B735" t="s">
         <v>63</v>
       </c>
-      <c r="C735" t="s">
-        <v>77</v>
-      </c>
-      <c r="D735" t="s">
-        <v>77</v>
-      </c>
-      <c r="E735" t="s">
-        <v>77</v>
-      </c>
-      <c r="F735" t="s">
-        <v>77</v>
+      <c r="C735">
+        <v>1</v>
+      </c>
+      <c r="D735">
+        <v>1</v>
+      </c>
+      <c r="E735">
+        <v>1</v>
+      </c>
+      <c r="F735">
+        <v>1</v>
       </c>
     </row>
     <row r="736" spans="1:6">

</xml_diff>

<commit_message>
updating yes button and dropdown menu background
</commit_message>
<xml_diff>
--- a/app/outputs/partner-solver-init-weights.xlsx
+++ b/app/outputs/partner-solver-init-weights.xlsx
@@ -1278,17 +1278,17 @@
       <c r="B34" t="s">
         <v>45</v>
       </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="F34">
-        <v>1</v>
+      <c r="C34" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" t="s">
+        <v>77</v>
+      </c>
+      <c r="F34" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2818,17 +2818,17 @@
       <c r="B111" t="s">
         <v>47</v>
       </c>
-      <c r="C111" t="s">
-        <v>77</v>
-      </c>
-      <c r="D111" t="s">
-        <v>77</v>
-      </c>
-      <c r="E111" t="s">
-        <v>77</v>
-      </c>
-      <c r="F111" t="s">
-        <v>77</v>
+      <c r="C111">
+        <v>1</v>
+      </c>
+      <c r="D111">
+        <v>1</v>
+      </c>
+      <c r="E111">
+        <v>1</v>
+      </c>
+      <c r="F111">
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:6">

</xml_diff>

<commit_message>
fixed tech weight error
</commit_message>
<xml_diff>
--- a/app/outputs/partner-solver-init-weights.xlsx
+++ b/app/outputs/partner-solver-init-weights.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6720" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6720" uniqueCount="130">
   <si>
     <t>Org_y</t>
   </si>
@@ -402,6 +402,9 @@
   <si>
     <t>1</t>
   </si>
+  <si>
+    <t>3</t>
+  </si>
 </sst>
 </file>
 
@@ -2312,20 +2315,20 @@
       <c r="B68" t="s">
         <v>85</v>
       </c>
-      <c r="C68" t="s">
-        <v>128</v>
-      </c>
-      <c r="D68" t="s">
-        <v>128</v>
-      </c>
-      <c r="E68" t="s">
-        <v>128</v>
-      </c>
-      <c r="F68" t="s">
-        <v>128</v>
-      </c>
-      <c r="G68" t="s">
-        <v>128</v>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68">
+        <v>1</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -18067,20 +18070,20 @@
       <c r="B753" t="s">
         <v>94</v>
       </c>
-      <c r="C753">
-        <v>1</v>
-      </c>
-      <c r="D753">
-        <v>1</v>
-      </c>
-      <c r="E753">
-        <v>1</v>
-      </c>
-      <c r="F753">
-        <v>1</v>
-      </c>
-      <c r="G753">
-        <v>1</v>
+      <c r="C753" t="s">
+        <v>128</v>
+      </c>
+      <c r="D753" t="s">
+        <v>128</v>
+      </c>
+      <c r="E753" t="s">
+        <v>128</v>
+      </c>
+      <c r="F753" t="s">
+        <v>128</v>
+      </c>
+      <c r="G753" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="754" spans="1:7">

</xml_diff>

<commit_message>
increased number of parnters displayed to 50
</commit_message>
<xml_diff>
--- a/app/outputs/partner-solver-init-weights.xlsx
+++ b/app/outputs/partner-solver-init-weights.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6720" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6720" uniqueCount="130">
   <si>
     <t>Org_y</t>
   </si>
@@ -400,6 +400,9 @@
     <t>eggXYt</t>
   </si>
   <si>
+    <t>1.0</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
 </sst>
@@ -1208,20 +1211,20 @@
       <c r="B20" t="s">
         <v>85</v>
       </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
+      <c r="C20" t="s">
+        <v>128</v>
+      </c>
+      <c r="D20" t="s">
+        <v>129</v>
+      </c>
+      <c r="E20" t="s">
+        <v>129</v>
+      </c>
+      <c r="F20" t="s">
+        <v>129</v>
+      </c>
+      <c r="G20" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -3186,9 +3189,6 @@
       <c r="B106" t="s">
         <v>86</v>
       </c>
-      <c r="C106">
-        <v>1</v>
-      </c>
       <c r="D106">
         <v>1</v>
       </c>
@@ -4107,7 +4107,7 @@
         <v>86</v>
       </c>
       <c r="C146">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D146">
         <v>1</v>
@@ -12156,20 +12156,20 @@
       <c r="B496" t="s">
         <v>91</v>
       </c>
-      <c r="C496" t="s">
-        <v>128</v>
-      </c>
-      <c r="D496" t="s">
-        <v>128</v>
-      </c>
-      <c r="E496" t="s">
-        <v>128</v>
-      </c>
-      <c r="F496" t="s">
-        <v>128</v>
-      </c>
-      <c r="G496" t="s">
-        <v>128</v>
+      <c r="C496">
+        <v>1</v>
+      </c>
+      <c r="D496">
+        <v>1</v>
+      </c>
+      <c r="E496">
+        <v>1</v>
+      </c>
+      <c r="F496">
+        <v>1</v>
+      </c>
+      <c r="G496">
+        <v>1</v>
       </c>
     </row>
     <row r="497" spans="1:7">
@@ -17321,7 +17321,7 @@
         <v>1</v>
       </c>
       <c r="G720">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="721" spans="1:7">
@@ -17873,7 +17873,7 @@
         <v>1</v>
       </c>
       <c r="G744">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="745" spans="1:7">
@@ -18287,7 +18287,7 @@
         <v>1</v>
       </c>
       <c r="G762">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="763" spans="1:7">
@@ -47175,7 +47175,7 @@
         <v>1</v>
       </c>
       <c r="G2018">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2019" spans="1:7">

</xml_diff>

<commit_message>
eliminated individual partner plot, added stacked bar chart for main plot, added history tracking xlsx file
</commit_message>
<xml_diff>
--- a/app/outputs/partner-solver-init-weights.xlsx
+++ b/app/outputs/partner-solver-init-weights.xlsx
@@ -1211,20 +1211,20 @@
       <c r="B20" t="s">
         <v>85</v>
       </c>
-      <c r="C20" t="s">
-        <v>128</v>
-      </c>
-      <c r="D20" t="s">
-        <v>129</v>
-      </c>
-      <c r="E20" t="s">
-        <v>129</v>
-      </c>
-      <c r="F20" t="s">
-        <v>129</v>
-      </c>
-      <c r="G20" t="s">
-        <v>129</v>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -2315,20 +2315,20 @@
       <c r="B68" t="s">
         <v>85</v>
       </c>
-      <c r="C68">
-        <v>1</v>
-      </c>
-      <c r="D68">
-        <v>1</v>
-      </c>
-      <c r="E68">
-        <v>1</v>
-      </c>
-      <c r="F68">
-        <v>1</v>
-      </c>
-      <c r="G68">
-        <v>1</v>
+      <c r="C68" t="s">
+        <v>128</v>
+      </c>
+      <c r="D68" t="s">
+        <v>129</v>
+      </c>
+      <c r="E68" t="s">
+        <v>129</v>
+      </c>
+      <c r="F68" t="s">
+        <v>129</v>
+      </c>
+      <c r="G68" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="69" spans="1:7">

</xml_diff>